<commit_message>
Finales Zeiblatt Update - EOD
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Thomas Rienoeßl.xlsx
+++ b/Zeitblaetter/Thomas Rienoeßl.xlsx
@@ -473,7 +473,7 @@
         <v>42669</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>3</v>
+        <v>4.25</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>17</v>
@@ -518,7 +518,7 @@
       </c>
       <c r="B36" s="3" t="n">
         <f aca="false">SUM(B5:B34)</f>
-        <v>39.25</v>
+        <v>40.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>